<commit_message>
Questions from Iris checks
</commit_message>
<xml_diff>
--- a/Data/Iris_inputs_v4.xlsx
+++ b/Data/Iris_inputs_v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A376E2B-D6B6-4DF0-B591-66288E37ED64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40B7612-674A-46E9-96AE-746455481265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47970" yWindow="5160" windowWidth="17280" windowHeight="9075" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iris_original" sheetId="2" r:id="rId1"/>
@@ -1436,6 +1436,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1471,66 +1531,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1900,8 +1900,8 @@
   <dimension ref="A1:P121"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
+      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1919,14 +1919,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
     </row>
     <row r="2" spans="1:11">
       <c r="B2" s="33"/>
@@ -1960,7 +1960,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="111" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1984,7 +1984,7 @@
       <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="92"/>
+      <c r="A5" s="112"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="K5" s="79"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="92"/>
+      <c r="A6" s="112"/>
       <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="K6" s="87"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="92"/>
+      <c r="A7" s="112"/>
       <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
@@ -2067,7 +2067,7 @@
       <c r="K7" s="87"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="92"/>
+      <c r="A8" s="112"/>
       <c r="B8" s="8" t="s">
         <v>154</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="H8" s="57"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="92"/>
+      <c r="A9" s="112"/>
       <c r="B9" s="8" t="s">
         <v>65</v>
       </c>
@@ -2115,7 +2115,7 @@
       <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="92"/>
+      <c r="A10" s="112"/>
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
@@ -2206,7 +2206,7 @@
       <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:11" s="35" customFormat="1" ht="14.7" customHeight="1">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="113" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="46" t="s">
@@ -2236,7 +2236,7 @@
       <c r="K14" s="67"/>
     </row>
     <row r="15" spans="1:11" s="35" customFormat="1">
-      <c r="A15" s="94"/>
+      <c r="A15" s="114"/>
       <c r="B15" s="46" t="s">
         <v>74</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="K15" s="68"/>
     </row>
     <row r="16" spans="1:11" s="35" customFormat="1">
-      <c r="A16" s="94"/>
+      <c r="A16" s="114"/>
       <c r="B16" s="46" t="s">
         <v>75</v>
       </c>
@@ -2292,7 +2292,7 @@
       <c r="K16" s="68"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="95" t="s">
+      <c r="A17" s="115" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -2318,7 +2318,7 @@
       <c r="H17" s="85"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="95"/>
+      <c r="A18" s="115"/>
       <c r="B18" s="25" t="s">
         <v>76</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="95"/>
+      <c r="A19" s="115"/>
       <c r="B19" s="25" t="s">
         <v>79</v>
       </c>
@@ -2366,7 +2366,7 @@
       <c r="H19" s="69"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="95"/>
+      <c r="A20" s="115"/>
       <c r="B20" s="25" t="s">
         <v>80</v>
       </c>
@@ -2390,7 +2390,7 @@
       <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="95"/>
+      <c r="A21" s="115"/>
       <c r="B21" s="25" t="s">
         <v>86</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="H21" s="49"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="95"/>
+      <c r="A22" s="115"/>
       <c r="B22" s="25" t="s">
         <v>87</v>
       </c>
@@ -2438,7 +2438,7 @@
       <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="95"/>
+      <c r="A23" s="115"/>
       <c r="B23" s="25" t="s">
         <v>90</v>
       </c>
@@ -2462,7 +2462,7 @@
       <c r="H23" s="49"/>
     </row>
     <row r="24" spans="1:15" ht="14.4" customHeight="1">
-      <c r="A24" s="96" t="s">
+      <c r="A24" s="116" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -2486,7 +2486,7 @@
       <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:15" ht="14.4" customHeight="1">
-      <c r="A25" s="97"/>
+      <c r="A25" s="117"/>
       <c r="B25" s="9" t="s">
         <v>12</v>
       </c>
@@ -2508,7 +2508,7 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="97"/>
+      <c r="A26" s="117"/>
       <c r="B26" s="9" t="s">
         <v>13</v>
       </c>
@@ -2530,7 +2530,7 @@
       <c r="H26" s="49"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="97"/>
+      <c r="A27" s="117"/>
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
@@ -2552,7 +2552,7 @@
       <c r="H27" s="49"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="97"/>
+      <c r="A28" s="117"/>
       <c r="B28" s="9" t="s">
         <v>14</v>
       </c>
@@ -2574,7 +2574,7 @@
       <c r="H28" s="49"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="97"/>
+      <c r="A29" s="117"/>
       <c r="B29" s="9" t="s">
         <v>15</v>
       </c>
@@ -2596,7 +2596,7 @@
       <c r="H29" s="49"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="97"/>
+      <c r="A30" s="117"/>
       <c r="B30" s="36" t="s">
         <v>16</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="H30" s="49"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="97"/>
+      <c r="A31" s="117"/>
       <c r="B31" s="36" t="s">
         <v>17</v>
       </c>
@@ -2640,7 +2640,7 @@
       <c r="H31" s="50"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="97"/>
+      <c r="A32" s="117"/>
       <c r="B32" s="36" t="s">
         <v>18</v>
       </c>
@@ -2660,14 +2660,14 @@
         <v>114</v>
       </c>
       <c r="H32" s="50"/>
-      <c r="M32" s="101" t="s">
+      <c r="M32" s="92" t="s">
         <v>205</v>
       </c>
-      <c r="N32" s="102"/>
-      <c r="O32" s="103"/>
+      <c r="N32" s="93"/>
+      <c r="O32" s="94"/>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="97"/>
+      <c r="A33" s="117"/>
       <c r="B33" s="36" t="s">
         <v>22</v>
       </c>
@@ -2687,14 +2687,14 @@
         <v>115</v>
       </c>
       <c r="H33" s="80"/>
-      <c r="M33" s="112" t="s">
+      <c r="M33" s="103" t="s">
         <v>207</v>
       </c>
-      <c r="N33" s="114"/>
-      <c r="O33" s="113"/>
+      <c r="N33" s="105"/>
+      <c r="O33" s="104"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="97"/>
+      <c r="A34" s="117"/>
       <c r="B34" s="36" t="s">
         <v>19</v>
       </c>
@@ -2725,7 +2725,7 @@
       </c>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="97"/>
+      <c r="A35" s="117"/>
       <c r="B35" s="36" t="s">
         <v>20</v>
       </c>
@@ -2757,7 +2757,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="100" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="51" t="s">
@@ -2785,14 +2785,14 @@
       <c r="I36" s="68"/>
       <c r="J36" s="68"/>
       <c r="K36" s="68"/>
-      <c r="M36" s="112" t="s">
+      <c r="M36" s="103" t="s">
         <v>206</v>
       </c>
-      <c r="N36" s="114"/>
-      <c r="O36" s="113"/>
+      <c r="N36" s="105"/>
+      <c r="O36" s="104"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="110"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="51" t="s">
         <v>27</v>
       </c>
@@ -2829,7 +2829,7 @@
       </c>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="110"/>
+      <c r="A38" s="101"/>
       <c r="B38" s="51" t="s">
         <v>28</v>
       </c>
@@ -2861,13 +2861,13 @@
       <c r="N38" s="49">
         <v>1500</v>
       </c>
-      <c r="O38" s="115">
+      <c r="O38" s="106">
         <f>N38*M38+M39*N39+M40*N40</f>
         <v>2805</v>
       </c>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="110"/>
+      <c r="A39" s="101"/>
       <c r="B39" s="51" t="s">
         <v>29</v>
       </c>
@@ -2899,10 +2899,10 @@
       <c r="N39" s="49">
         <v>6500</v>
       </c>
-      <c r="O39" s="116"/>
+      <c r="O39" s="107"/>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="111"/>
+      <c r="A40" s="102"/>
       <c r="B40" s="14" t="s">
         <v>165</v>
       </c>
@@ -2930,10 +2930,10 @@
       <c r="N40" s="49">
         <v>500</v>
       </c>
-      <c r="O40" s="117"/>
+      <c r="O40" s="108"/>
     </row>
     <row r="41" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A41" s="106" t="s">
+      <c r="A41" s="97" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="17" t="s">
@@ -2959,7 +2959,7 @@
       <c r="H41" s="49"/>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="107"/>
+      <c r="A42" s="98"/>
       <c r="B42" s="17" t="s">
         <v>33</v>
       </c>
@@ -2981,13 +2981,13 @@
         <v>123</v>
       </c>
       <c r="H42" s="49"/>
-      <c r="M42" s="112" t="s">
+      <c r="M42" s="103" t="s">
         <v>191</v>
       </c>
-      <c r="N42" s="113"/>
+      <c r="N42" s="104"/>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="107"/>
+      <c r="A43" s="98"/>
       <c r="B43" s="17" t="s">
         <v>34</v>
       </c>
@@ -3021,7 +3021,7 @@
       </c>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="107"/>
+      <c r="A44" s="98"/>
       <c r="B44" s="17" t="s">
         <v>35</v>
       </c>
@@ -3056,7 +3056,7 @@
       </c>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="107"/>
+      <c r="A45" s="98"/>
       <c r="B45" s="17" t="s">
         <v>36</v>
       </c>
@@ -3091,7 +3091,7 @@
       </c>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="107"/>
+      <c r="A46" s="98"/>
       <c r="B46" s="17" t="s">
         <v>37</v>
       </c>
@@ -3115,7 +3115,7 @@
       <c r="H46" s="49"/>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="108"/>
+      <c r="A47" s="99"/>
       <c r="B47" s="17" t="s">
         <v>151</v>
       </c>
@@ -3137,15 +3137,15 @@
         <v>162</v>
       </c>
       <c r="H47" s="49"/>
-      <c r="M47" s="112" t="s">
+      <c r="M47" s="103" t="s">
         <v>192</v>
       </c>
-      <c r="N47" s="114"/>
-      <c r="O47" s="114"/>
-      <c r="P47" s="113"/>
+      <c r="N47" s="105"/>
+      <c r="O47" s="105"/>
+      <c r="P47" s="104"/>
     </row>
     <row r="48" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A48" s="98" t="s">
+      <c r="A48" s="118" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="20" t="s">
@@ -3181,7 +3181,7 @@
       </c>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="99"/>
+      <c r="A49" s="119"/>
       <c r="B49" s="20" t="s">
         <v>171</v>
       </c>
@@ -3221,7 +3221,7 @@
       </c>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="99"/>
+      <c r="A50" s="119"/>
       <c r="B50" s="20" t="s">
         <v>173</v>
       </c>
@@ -3263,7 +3263,7 @@
       </c>
     </row>
     <row r="51" spans="1:16">
-      <c r="A51" s="99"/>
+      <c r="A51" s="119"/>
       <c r="B51" s="20" t="s">
         <v>213</v>
       </c>
@@ -3295,7 +3295,7 @@
       <c r="P51" s="59"/>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="99"/>
+      <c r="A52" s="119"/>
       <c r="B52" s="20" t="s">
         <v>212</v>
       </c>
@@ -3337,7 +3337,7 @@
       </c>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" s="99"/>
+      <c r="A53" s="119"/>
       <c r="B53" s="20" t="s">
         <v>217</v>
       </c>
@@ -3379,7 +3379,7 @@
       </c>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="99"/>
+      <c r="A54" s="119"/>
       <c r="B54" s="20" t="s">
         <v>170</v>
       </c>
@@ -3406,7 +3406,7 @@
       <c r="K54" s="88"/>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="99"/>
+      <c r="A55" s="119"/>
       <c r="B55" s="20" t="s">
         <v>174</v>
       </c>
@@ -3442,7 +3442,7 @@
       </c>
     </row>
     <row r="56" spans="1:16">
-      <c r="A56" s="99"/>
+      <c r="A56" s="119"/>
       <c r="B56" s="23" t="s">
         <v>208</v>
       </c>
@@ -3479,7 +3479,7 @@
       </c>
     </row>
     <row r="57" spans="1:16">
-      <c r="A57" s="99"/>
+      <c r="A57" s="119"/>
       <c r="B57" s="23" t="s">
         <v>209</v>
       </c>
@@ -3515,7 +3515,7 @@
       </c>
     </row>
     <row r="58" spans="1:16">
-      <c r="A58" s="99"/>
+      <c r="A58" s="119"/>
       <c r="B58" s="23" t="s">
         <v>163</v>
       </c>
@@ -3548,7 +3548,7 @@
       </c>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="99"/>
+      <c r="A59" s="119"/>
       <c r="B59" s="23" t="s">
         <v>164</v>
       </c>
@@ -3571,7 +3571,7 @@
       <c r="H59" s="49"/>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="99"/>
+      <c r="A60" s="119"/>
       <c r="B60" s="23" t="s">
         <v>221</v>
       </c>
@@ -3593,7 +3593,7 @@
       <c r="H60" s="73"/>
     </row>
     <row r="61" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A61" s="99"/>
+      <c r="A61" s="119"/>
       <c r="B61" s="41" t="s">
         <v>41</v>
       </c>
@@ -3625,7 +3625,7 @@
       </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" s="99"/>
+      <c r="A62" s="119"/>
       <c r="B62" s="41" t="s">
         <v>42</v>
       </c>
@@ -3657,7 +3657,7 @@
       </c>
     </row>
     <row r="63" spans="1:16">
-      <c r="A63" s="99"/>
+      <c r="A63" s="119"/>
       <c r="B63" s="41" t="s">
         <v>92</v>
       </c>
@@ -3689,7 +3689,7 @@
       </c>
     </row>
     <row r="64" spans="1:16">
-      <c r="A64" s="100"/>
+      <c r="A64" s="120"/>
       <c r="B64" s="41" t="s">
         <v>93</v>
       </c>
@@ -3721,7 +3721,7 @@
       </c>
     </row>
     <row r="65" spans="1:13">
-      <c r="A65" s="120"/>
+      <c r="A65" s="91"/>
       <c r="B65" s="41" t="s">
         <v>225</v>
       </c>
@@ -3743,7 +3743,7 @@
       <c r="H65" s="81"/>
     </row>
     <row r="66" spans="1:13" ht="14.4" customHeight="1">
-      <c r="A66" s="89" t="s">
+      <c r="A66" s="109" t="s">
         <v>49</v>
       </c>
       <c r="B66" s="55" t="s">
@@ -3767,7 +3767,7 @@
       <c r="H66" s="83"/>
     </row>
     <row r="67" spans="1:13">
-      <c r="A67" s="90"/>
+      <c r="A67" s="110"/>
       <c r="B67" s="55" t="s">
         <v>59</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="H67" s="84"/>
     </row>
     <row r="68" spans="1:13">
-      <c r="A68" s="90"/>
+      <c r="A68" s="110"/>
       <c r="B68" s="55" t="s">
         <v>51</v>
       </c>
@@ -3811,7 +3811,7 @@
       <c r="H68" s="84"/>
     </row>
     <row r="69" spans="1:13">
-      <c r="A69" s="90"/>
+      <c r="A69" s="110"/>
       <c r="B69" s="55" t="s">
         <v>52</v>
       </c>
@@ -3833,7 +3833,7 @@
       <c r="H69" s="84"/>
     </row>
     <row r="70" spans="1:13">
-      <c r="A70" s="90"/>
+      <c r="A70" s="110"/>
       <c r="B70" s="55" t="s">
         <v>53</v>
       </c>
@@ -3855,7 +3855,7 @@
       <c r="H70" s="84"/>
     </row>
     <row r="71" spans="1:13">
-      <c r="A71" s="90"/>
+      <c r="A71" s="110"/>
       <c r="B71" s="55" t="s">
         <v>94</v>
       </c>
@@ -3877,7 +3877,7 @@
       <c r="H71" s="84"/>
     </row>
     <row r="72" spans="1:13">
-      <c r="A72" s="90"/>
+      <c r="A72" s="110"/>
       <c r="B72" s="55" t="s">
         <v>54</v>
       </c>
@@ -3900,7 +3900,7 @@
       <c r="M72" s="13"/>
     </row>
     <row r="73" spans="1:13">
-      <c r="A73" s="90"/>
+      <c r="A73" s="110"/>
       <c r="B73" s="55" t="s">
         <v>60</v>
       </c>
@@ -3923,7 +3923,7 @@
       <c r="M73" s="13"/>
     </row>
     <row r="74" spans="1:13">
-      <c r="A74" s="90"/>
+      <c r="A74" s="110"/>
       <c r="B74" s="55" t="s">
         <v>55</v>
       </c>
@@ -3946,7 +3946,7 @@
       <c r="M74" s="13"/>
     </row>
     <row r="75" spans="1:13">
-      <c r="A75" s="90"/>
+      <c r="A75" s="110"/>
       <c r="B75" s="55" t="s">
         <v>56</v>
       </c>
@@ -3969,7 +3969,7 @@
       <c r="M75" s="13"/>
     </row>
     <row r="76" spans="1:13">
-      <c r="A76" s="90"/>
+      <c r="A76" s="110"/>
       <c r="B76" s="55" t="s">
         <v>57</v>
       </c>
@@ -3992,7 +3992,7 @@
       <c r="M76" s="13"/>
     </row>
     <row r="77" spans="1:13">
-      <c r="A77" s="90"/>
+      <c r="A77" s="110"/>
       <c r="B77" s="55" t="s">
         <v>96</v>
       </c>
@@ -4015,7 +4015,7 @@
       <c r="M77" s="13"/>
     </row>
     <row r="78" spans="1:13">
-      <c r="A78" s="90"/>
+      <c r="A78" s="110"/>
       <c r="B78" s="55" t="s">
         <v>58</v>
       </c>
@@ -4037,7 +4037,7 @@
       <c r="H78" s="84"/>
     </row>
     <row r="79" spans="1:13">
-      <c r="A79" s="90"/>
+      <c r="A79" s="110"/>
       <c r="B79" s="55" t="s">
         <v>61</v>
       </c>
@@ -4059,7 +4059,7 @@
       <c r="H79" s="84"/>
     </row>
     <row r="80" spans="1:13">
-      <c r="A80" s="90"/>
+      <c r="A80" s="110"/>
       <c r="B80" s="55" t="s">
         <v>62</v>
       </c>
@@ -4081,7 +4081,7 @@
       <c r="H80" s="84"/>
     </row>
     <row r="81" spans="1:13">
-      <c r="A81" s="90"/>
+      <c r="A81" s="110"/>
       <c r="B81" s="55" t="s">
         <v>63</v>
       </c>
@@ -4103,7 +4103,7 @@
       <c r="H81" s="84"/>
     </row>
     <row r="82" spans="1:13">
-      <c r="A82" s="90"/>
+      <c r="A82" s="110"/>
       <c r="B82" s="55" t="s">
         <v>64</v>
       </c>
@@ -4125,7 +4125,7 @@
       <c r="H82" s="84"/>
     </row>
     <row r="83" spans="1:13">
-      <c r="A83" s="90"/>
+      <c r="A83" s="110"/>
       <c r="B83" s="55" t="s">
         <v>95</v>
       </c>
@@ -4196,6 +4196,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A66:A83"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A24:A35"/>
+    <mergeCell ref="A48:A64"/>
     <mergeCell ref="M32:O32"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A41:A47"/>
@@ -4205,12 +4211,6 @@
     <mergeCell ref="O38:O40"/>
     <mergeCell ref="M33:O33"/>
     <mergeCell ref="M36:O36"/>
-    <mergeCell ref="A66:A83"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A24:A35"/>
-    <mergeCell ref="A48:A64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4222,8 +4222,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22540C2-7758-43CC-8CAC-337C735D93EA}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4237,14 +4240,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="95" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="4" t="s">
@@ -4270,7 +4273,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="111" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -4294,7 +4297,7 @@
       <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="92"/>
+      <c r="A5" s="112"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4318,7 +4321,7 @@
       <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="92"/>
+      <c r="A6" s="112"/>
       <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
@@ -4343,7 +4346,7 @@
       <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="92"/>
+      <c r="A7" s="112"/>
       <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
@@ -4351,11 +4354,11 @@
         <f>31.5/60</f>
         <v>0.52500000000000002</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="75">
         <f t="shared" si="0"/>
         <v>0.47250000000000003</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="75">
         <f t="shared" si="1"/>
         <v>0.57750000000000012</v>
       </c>
@@ -4368,18 +4371,18 @@
       <c r="H7" s="49"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="92"/>
+      <c r="A8" s="112"/>
       <c r="B8" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C8" s="70">
         <v>380</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="75">
         <f t="shared" si="0"/>
         <v>342</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="75">
         <f t="shared" si="1"/>
         <v>418.00000000000006</v>
       </c>
@@ -4392,18 +4395,18 @@
       <c r="H8" s="57"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="92"/>
+      <c r="A9" s="112"/>
       <c r="B9" s="8" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="75">
         <v>30</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="75">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="75">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
@@ -4416,7 +4419,7 @@
       <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="92"/>
+      <c r="A10" s="112"/>
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
@@ -4424,11 +4427,11 @@
         <f>747</f>
         <v>747</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="75">
         <f t="shared" si="0"/>
         <v>672.30000000000007</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="75">
         <f t="shared" si="1"/>
         <v>821.7</v>
       </c>
@@ -4448,11 +4451,11 @@
       <c r="C11" s="75">
         <v>10</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="75">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="75">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -4470,11 +4473,11 @@
       <c r="C12" s="75">
         <v>20</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="75">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="75">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
@@ -4492,11 +4495,11 @@
       <c r="C13" s="75">
         <v>70</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="75">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="75">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
@@ -4507,7 +4510,7 @@
       <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="113" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="46" t="s">
@@ -4534,7 +4537,7 @@
       <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="94"/>
+      <c r="A15" s="114"/>
       <c r="B15" s="46" t="s">
         <v>74</v>
       </c>
@@ -4559,7 +4562,7 @@
       <c r="H15" s="83"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="94"/>
+      <c r="A16" s="114"/>
       <c r="B16" s="46" t="s">
         <v>75</v>
       </c>
@@ -4584,7 +4587,7 @@
       <c r="H16" s="84"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="95" t="s">
+      <c r="A17" s="115" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -4610,7 +4613,7 @@
       <c r="H17" s="85"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="95"/>
+      <c r="A18" s="115"/>
       <c r="B18" s="25" t="s">
         <v>76</v>
       </c>
@@ -4634,7 +4637,7 @@
       <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="95"/>
+      <c r="A19" s="115"/>
       <c r="B19" s="25" t="s">
         <v>79</v>
       </c>
@@ -4658,7 +4661,7 @@
       <c r="H19" s="69"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="95"/>
+      <c r="A20" s="115"/>
       <c r="B20" s="25" t="s">
         <v>80</v>
       </c>
@@ -4682,7 +4685,7 @@
       <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="95"/>
+      <c r="A21" s="115"/>
       <c r="B21" s="25" t="s">
         <v>86</v>
       </c>
@@ -4706,7 +4709,7 @@
       <c r="H21" s="49"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="95"/>
+      <c r="A22" s="115"/>
       <c r="B22" s="25" t="s">
         <v>87</v>
       </c>
@@ -4730,7 +4733,7 @@
       <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="95"/>
+      <c r="A23" s="115"/>
       <c r="B23" s="25" t="s">
         <v>90</v>
       </c>
@@ -4754,7 +4757,7 @@
       <c r="H23" s="49"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="96" t="s">
+      <c r="A24" s="116" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -4778,7 +4781,7 @@
       <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="97"/>
+      <c r="A25" s="117"/>
       <c r="B25" s="9" t="s">
         <v>12</v>
       </c>
@@ -4800,7 +4803,7 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="97"/>
+      <c r="A26" s="117"/>
       <c r="B26" s="9" t="s">
         <v>13</v>
       </c>
@@ -4822,7 +4825,7 @@
       <c r="H26" s="49"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="97"/>
+      <c r="A27" s="117"/>
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
@@ -4844,7 +4847,7 @@
       <c r="H27" s="49"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="97"/>
+      <c r="A28" s="117"/>
       <c r="B28" s="9" t="s">
         <v>14</v>
       </c>
@@ -4866,7 +4869,7 @@
       <c r="H28" s="49"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="97"/>
+      <c r="A29" s="117"/>
       <c r="B29" s="9" t="s">
         <v>15</v>
       </c>
@@ -4888,7 +4891,7 @@
       <c r="H29" s="49"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="97"/>
+      <c r="A30" s="117"/>
       <c r="B30" s="36" t="s">
         <v>16</v>
       </c>
@@ -4910,7 +4913,7 @@
       <c r="H30" s="49"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="97"/>
+      <c r="A31" s="117"/>
       <c r="B31" s="36" t="s">
         <v>17</v>
       </c>
@@ -4932,7 +4935,7 @@
       <c r="H31" s="50"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="97"/>
+      <c r="A32" s="117"/>
       <c r="B32" s="36" t="s">
         <v>18</v>
       </c>
@@ -4954,7 +4957,7 @@
       <c r="H32" s="50"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="97"/>
+      <c r="A33" s="117"/>
       <c r="B33" s="36" t="s">
         <v>22</v>
       </c>
@@ -4976,7 +4979,7 @@
       <c r="H33" s="80"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="97"/>
+      <c r="A34" s="117"/>
       <c r="B34" s="36" t="s">
         <v>19</v>
       </c>
@@ -4998,7 +5001,7 @@
       <c r="H34" s="81"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="97"/>
+      <c r="A35" s="117"/>
       <c r="B35" s="36" t="s">
         <v>20</v>
       </c>
@@ -5020,7 +5023,7 @@
       <c r="H35" s="81"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="100" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="51" t="s">
@@ -5047,7 +5050,7 @@
       <c r="H36" s="82"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="110"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="51" t="s">
         <v>27</v>
       </c>
@@ -5072,7 +5075,7 @@
       <c r="H37" s="80"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="110"/>
+      <c r="A38" s="101"/>
       <c r="B38" s="51" t="s">
         <v>28</v>
       </c>
@@ -5097,7 +5100,7 @@
       <c r="H38" s="81"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="110"/>
+      <c r="A39" s="101"/>
       <c r="B39" s="51" t="s">
         <v>29</v>
       </c>
@@ -5122,7 +5125,7 @@
       <c r="H39" s="81"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="111"/>
+      <c r="A40" s="102"/>
       <c r="B40" s="14" t="s">
         <v>165</v>
       </c>
@@ -5146,7 +5149,7 @@
       <c r="H40" s="82"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="106" t="s">
+      <c r="A41" s="97" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="17" t="s">
@@ -5172,7 +5175,7 @@
       <c r="H41" s="49"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="107"/>
+      <c r="A42" s="98"/>
       <c r="B42" s="17" t="s">
         <v>33</v>
       </c>
@@ -5196,7 +5199,7 @@
       <c r="H42" s="49"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="107"/>
+      <c r="A43" s="98"/>
       <c r="B43" s="17" t="s">
         <v>34</v>
       </c>
@@ -5220,7 +5223,7 @@
       <c r="H43" s="49"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="107"/>
+      <c r="A44" s="98"/>
       <c r="B44" s="17" t="s">
         <v>35</v>
       </c>
@@ -5244,7 +5247,7 @@
       <c r="H44" s="49"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="107"/>
+      <c r="A45" s="98"/>
       <c r="B45" s="17" t="s">
         <v>36</v>
       </c>
@@ -5268,7 +5271,7 @@
       <c r="H45" s="49"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="107"/>
+      <c r="A46" s="98"/>
       <c r="B46" s="17" t="s">
         <v>37</v>
       </c>
@@ -5292,7 +5295,7 @@
       <c r="H46" s="49"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="108"/>
+      <c r="A47" s="99"/>
       <c r="B47" s="17" t="s">
         <v>151</v>
       </c>
@@ -5316,7 +5319,7 @@
       <c r="H47" s="49"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="98" t="s">
+      <c r="A48" s="118" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="20" t="s">
@@ -5343,7 +5346,7 @@
       <c r="H48" s="49"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="99"/>
+      <c r="A49" s="119"/>
       <c r="B49" s="20" t="s">
         <v>171</v>
       </c>
@@ -5368,7 +5371,7 @@
       <c r="H49" s="80"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="99"/>
+      <c r="A50" s="119"/>
       <c r="B50" s="20" t="s">
         <v>173</v>
       </c>
@@ -5393,7 +5396,7 @@
       <c r="H50" s="81"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="99"/>
+      <c r="A51" s="119"/>
       <c r="B51" s="20" t="s">
         <v>213</v>
       </c>
@@ -5418,7 +5421,7 @@
       <c r="H51" s="81"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="99"/>
+      <c r="A52" s="119"/>
       <c r="B52" s="20" t="s">
         <v>212</v>
       </c>
@@ -5443,7 +5446,7 @@
       <c r="H52" s="81"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="99"/>
+      <c r="A53" s="119"/>
       <c r="B53" s="20" t="s">
         <v>217</v>
       </c>
@@ -5468,7 +5471,7 @@
       <c r="H53" s="81"/>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="99"/>
+      <c r="A54" s="119"/>
       <c r="B54" s="20" t="s">
         <v>170</v>
       </c>
@@ -5492,7 +5495,7 @@
       <c r="H54" s="81"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="99"/>
+      <c r="A55" s="119"/>
       <c r="B55" s="20" t="s">
         <v>174</v>
       </c>
@@ -5516,7 +5519,7 @@
       <c r="H55" s="81"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="99"/>
+      <c r="A56" s="119"/>
       <c r="B56" s="23" t="s">
         <v>208</v>
       </c>
@@ -5541,7 +5544,7 @@
       <c r="H56" s="81"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="99"/>
+      <c r="A57" s="119"/>
       <c r="B57" s="23" t="s">
         <v>209</v>
       </c>
@@ -5565,7 +5568,7 @@
       <c r="H57" s="81"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="99"/>
+      <c r="A58" s="119"/>
       <c r="B58" s="23" t="s">
         <v>163</v>
       </c>
@@ -5590,7 +5593,7 @@
       <c r="H58" s="82"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="99"/>
+      <c r="A59" s="119"/>
       <c r="B59" s="23" t="s">
         <v>164</v>
       </c>
@@ -5613,7 +5616,7 @@
       <c r="H59" s="49"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="99"/>
+      <c r="A60" s="119"/>
       <c r="B60" s="23" t="s">
         <v>221</v>
       </c>
@@ -5635,7 +5638,7 @@
       <c r="H60" s="73"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="99"/>
+      <c r="A61" s="119"/>
       <c r="B61" s="41" t="s">
         <v>41</v>
       </c>
@@ -5659,7 +5662,7 @@
       <c r="H61" s="80"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="99"/>
+      <c r="A62" s="119"/>
       <c r="B62" s="41" t="s">
         <v>42</v>
       </c>
@@ -5683,7 +5686,7 @@
       <c r="H62" s="81"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="99"/>
+      <c r="A63" s="119"/>
       <c r="B63" s="41" t="s">
         <v>92</v>
       </c>
@@ -5707,7 +5710,7 @@
       <c r="H63" s="81"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="100"/>
+      <c r="A64" s="120"/>
       <c r="B64" s="41" t="s">
         <v>93</v>
       </c>
@@ -5731,7 +5734,7 @@
       <c r="H64" s="82"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="120"/>
+      <c r="A65" s="91"/>
       <c r="B65" s="41" t="s">
         <v>225</v>
       </c>
@@ -5753,7 +5756,7 @@
       <c r="H65" s="81"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="89" t="s">
+      <c r="A66" s="109" t="s">
         <v>49</v>
       </c>
       <c r="B66" s="55" t="s">
@@ -5777,7 +5780,7 @@
       <c r="H66" s="83"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="90"/>
+      <c r="A67" s="110"/>
       <c r="B67" s="55" t="s">
         <v>59</v>
       </c>
@@ -5799,7 +5802,7 @@
       <c r="H67" s="84"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="90"/>
+      <c r="A68" s="110"/>
       <c r="B68" s="55" t="s">
         <v>51</v>
       </c>
@@ -5821,7 +5824,7 @@
       <c r="H68" s="84"/>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="90"/>
+      <c r="A69" s="110"/>
       <c r="B69" s="55" t="s">
         <v>52</v>
       </c>
@@ -5843,7 +5846,7 @@
       <c r="H69" s="84"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="90"/>
+      <c r="A70" s="110"/>
       <c r="B70" s="55" t="s">
         <v>53</v>
       </c>
@@ -5865,7 +5868,7 @@
       <c r="H70" s="84"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="90"/>
+      <c r="A71" s="110"/>
       <c r="B71" s="55" t="s">
         <v>94</v>
       </c>
@@ -5887,7 +5890,7 @@
       <c r="H71" s="84"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="90"/>
+      <c r="A72" s="110"/>
       <c r="B72" s="55" t="s">
         <v>54</v>
       </c>
@@ -5909,7 +5912,7 @@
       <c r="H72" s="84"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="90"/>
+      <c r="A73" s="110"/>
       <c r="B73" s="55" t="s">
         <v>60</v>
       </c>
@@ -5931,7 +5934,7 @@
       <c r="H73" s="84"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="90"/>
+      <c r="A74" s="110"/>
       <c r="B74" s="55" t="s">
         <v>55</v>
       </c>
@@ -5953,7 +5956,7 @@
       <c r="H74" s="84"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="90"/>
+      <c r="A75" s="110"/>
       <c r="B75" s="55" t="s">
         <v>56</v>
       </c>
@@ -5975,7 +5978,7 @@
       <c r="H75" s="84"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="90"/>
+      <c r="A76" s="110"/>
       <c r="B76" s="55" t="s">
         <v>57</v>
       </c>
@@ -5997,7 +6000,7 @@
       <c r="H76" s="84"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="90"/>
+      <c r="A77" s="110"/>
       <c r="B77" s="55" t="s">
         <v>96</v>
       </c>
@@ -6019,7 +6022,7 @@
       <c r="H77" s="84"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="90"/>
+      <c r="A78" s="110"/>
       <c r="B78" s="55" t="s">
         <v>58</v>
       </c>
@@ -6041,7 +6044,7 @@
       <c r="H78" s="84"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="90"/>
+      <c r="A79" s="110"/>
       <c r="B79" s="55" t="s">
         <v>61</v>
       </c>
@@ -6063,7 +6066,7 @@
       <c r="H79" s="84"/>
     </row>
     <row r="80" spans="1:8">
-      <c r="A80" s="90"/>
+      <c r="A80" s="110"/>
       <c r="B80" s="55" t="s">
         <v>62</v>
       </c>
@@ -6085,7 +6088,7 @@
       <c r="H80" s="84"/>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="90"/>
+      <c r="A81" s="110"/>
       <c r="B81" s="55" t="s">
         <v>63</v>
       </c>
@@ -6107,7 +6110,7 @@
       <c r="H81" s="84"/>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="90"/>
+      <c r="A82" s="110"/>
       <c r="B82" s="55" t="s">
         <v>64</v>
       </c>
@@ -6129,7 +6132,7 @@
       <c r="H82" s="84"/>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="90"/>
+      <c r="A83" s="110"/>
       <c r="B83" s="55" t="s">
         <v>95</v>
       </c>
@@ -6172,7 +6175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FDFB89-F078-4F84-A115-0B27F39D5164}">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
@@ -6187,14 +6190,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="95" t="s">
         <v>224</v>
       </c>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
     </row>
     <row r="2" spans="1:8">
       <c r="B2" s="33"/>
@@ -6228,7 +6231,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="111" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -6252,7 +6255,7 @@
       <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="92"/>
+      <c r="A5" s="112"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -6260,11 +6263,11 @@
         <v>2044</v>
       </c>
       <c r="D5" s="31">
-        <f>0.9*C5</f>
+        <f t="shared" ref="D5:D36" si="0">0.9*C5</f>
         <v>1839.6000000000001</v>
       </c>
       <c r="E5" s="31">
-        <f>1.1*C5</f>
+        <f t="shared" ref="E5:E36" si="1">1.1*C5</f>
         <v>2248.4</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -6276,7 +6279,7 @@
       <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="92"/>
+      <c r="A6" s="112"/>
       <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
@@ -6285,11 +6288,11 @@
         <v>953</v>
       </c>
       <c r="D6" s="31">
-        <f>0.9*C6</f>
+        <f t="shared" si="0"/>
         <v>857.7</v>
       </c>
       <c r="E6" s="31">
-        <f>1.1*C6</f>
+        <f t="shared" si="1"/>
         <v>1048.3000000000002</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -6301,7 +6304,7 @@
       <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="92"/>
+      <c r="A7" s="112"/>
       <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
@@ -6310,11 +6313,11 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="D7" s="31">
-        <f>0.9*C7</f>
+        <f t="shared" si="0"/>
         <v>0.47250000000000003</v>
       </c>
       <c r="E7" s="31">
-        <f>1.1*C7</f>
+        <f t="shared" si="1"/>
         <v>0.57750000000000012</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -6326,7 +6329,7 @@
       <c r="H7" s="49"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="92"/>
+      <c r="A8" s="112"/>
       <c r="B8" s="8" t="s">
         <v>154</v>
       </c>
@@ -6334,11 +6337,11 @@
         <v>380</v>
       </c>
       <c r="D8" s="31">
-        <f>0.9*C8</f>
+        <f t="shared" si="0"/>
         <v>342</v>
       </c>
       <c r="E8" s="31">
-        <f>1.1*C8</f>
+        <f t="shared" si="1"/>
         <v>418.00000000000006</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -6350,7 +6353,7 @@
       <c r="H8" s="57"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="92"/>
+      <c r="A9" s="112"/>
       <c r="B9" s="8" t="s">
         <v>65</v>
       </c>
@@ -6358,11 +6361,11 @@
         <v>30</v>
       </c>
       <c r="D9" s="31">
-        <f>0.9*C9</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E9" s="31">
-        <f>1.1*C9</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -6374,7 +6377,7 @@
       <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="92"/>
+      <c r="A10" s="112"/>
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
@@ -6382,11 +6385,11 @@
         <v>747</v>
       </c>
       <c r="D10" s="31">
-        <f>0.9*C10</f>
+        <f t="shared" si="0"/>
         <v>672.30000000000007</v>
       </c>
       <c r="E10" s="31">
-        <f>1.1*C10</f>
+        <f t="shared" si="1"/>
         <v>821.7</v>
       </c>
       <c r="F10" s="45" t="s">
@@ -6406,11 +6409,11 @@
         <v>10</v>
       </c>
       <c r="D11" s="31">
-        <f>0.9*C11</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E11" s="31">
-        <f>1.1*C11</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F11" s="40"/>
@@ -6428,11 +6431,11 @@
         <v>20</v>
       </c>
       <c r="D12" s="31">
-        <f>0.9*C12</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="E12" s="31">
-        <f>1.1*C12</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="F12" s="40"/>
@@ -6450,11 +6453,11 @@
         <v>70</v>
       </c>
       <c r="D13" s="31">
-        <f>0.9*C13</f>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="E13" s="31">
-        <f>1.1*C13</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="F13" s="40"/>
@@ -6464,7 +6467,7 @@
       <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="113" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="46" t="s">
@@ -6475,11 +6478,11 @@
         <v>1499.1899999999998</v>
       </c>
       <c r="D14" s="47">
-        <f>0.9*C14</f>
+        <f t="shared" si="0"/>
         <v>1349.271</v>
       </c>
       <c r="E14" s="47">
-        <f>1.1*C14</f>
+        <f t="shared" si="1"/>
         <v>1649.1089999999999</v>
       </c>
       <c r="F14" s="48" t="s">
@@ -6491,7 +6494,7 @@
       <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="94"/>
+      <c r="A15" s="114"/>
       <c r="B15" s="46" t="s">
         <v>74</v>
       </c>
@@ -6500,11 +6503,11 @@
         <v>2.66</v>
       </c>
       <c r="D15" s="47">
-        <f>0.9*C15</f>
+        <f t="shared" si="0"/>
         <v>2.3940000000000001</v>
       </c>
       <c r="E15" s="47">
-        <f>1.1*C15</f>
+        <f t="shared" si="1"/>
         <v>2.9260000000000006</v>
       </c>
       <c r="F15" s="48" t="s">
@@ -6516,7 +6519,7 @@
       <c r="H15" s="83"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="94"/>
+      <c r="A16" s="114"/>
       <c r="B16" s="46" t="s">
         <v>75</v>
       </c>
@@ -6525,11 +6528,11 @@
         <v>10.5</v>
       </c>
       <c r="D16" s="47">
-        <f>0.9*C16</f>
+        <f t="shared" si="0"/>
         <v>9.4500000000000011</v>
       </c>
       <c r="E16" s="47">
-        <f>1.1*C16</f>
+        <f t="shared" si="1"/>
         <v>11.55</v>
       </c>
       <c r="F16" s="48" t="s">
@@ -6541,7 +6544,7 @@
       <c r="H16" s="84"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="95" t="s">
+      <c r="A17" s="115" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -6551,11 +6554,11 @@
         <v>48</v>
       </c>
       <c r="D17" s="26">
-        <f>0.9*C17</f>
+        <f t="shared" si="0"/>
         <v>43.2</v>
       </c>
       <c r="E17" s="26">
-        <f>1.1*C17</f>
+        <f t="shared" si="1"/>
         <v>52.800000000000004</v>
       </c>
       <c r="F17" s="27" t="s">
@@ -6567,7 +6570,7 @@
       <c r="H17" s="85"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="95"/>
+      <c r="A18" s="115"/>
       <c r="B18" s="25" t="s">
         <v>76</v>
       </c>
@@ -6575,11 +6578,11 @@
         <v>7</v>
       </c>
       <c r="D18" s="28">
-        <f>0.9*C18</f>
+        <f t="shared" si="0"/>
         <v>6.3</v>
       </c>
       <c r="E18" s="28">
-        <f>1.1*C18</f>
+        <f t="shared" si="1"/>
         <v>7.7000000000000011</v>
       </c>
       <c r="F18" s="27" t="s">
@@ -6591,7 +6594,7 @@
       <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="95"/>
+      <c r="A19" s="115"/>
       <c r="B19" s="25" t="s">
         <v>79</v>
       </c>
@@ -6599,11 +6602,11 @@
         <v>2250</v>
       </c>
       <c r="D19" s="28">
-        <f>0.9*C19</f>
+        <f t="shared" si="0"/>
         <v>2025</v>
       </c>
       <c r="E19" s="28">
-        <f>1.1*C19</f>
+        <f t="shared" si="1"/>
         <v>2475</v>
       </c>
       <c r="F19" s="27" t="s">
@@ -6615,7 +6618,7 @@
       <c r="H19" s="69"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="95"/>
+      <c r="A20" s="115"/>
       <c r="B20" s="25" t="s">
         <v>80</v>
       </c>
@@ -6623,11 +6626,11 @@
         <v>10</v>
       </c>
       <c r="D20" s="28">
-        <f>0.9*C20</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E20" s="28">
-        <f>1.1*C20</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F20" s="27" t="s">
@@ -6639,7 +6642,7 @@
       <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="95"/>
+      <c r="A21" s="115"/>
       <c r="B21" s="25" t="s">
         <v>86</v>
       </c>
@@ -6647,11 +6650,11 @@
         <v>3</v>
       </c>
       <c r="D21" s="28">
-        <f>0.9*C21</f>
+        <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
       <c r="E21" s="28">
-        <f>1.1*C21</f>
+        <f t="shared" si="1"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="F21" s="27" t="s">
@@ -6663,7 +6666,7 @@
       <c r="H21" s="49"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="95"/>
+      <c r="A22" s="115"/>
       <c r="B22" s="25" t="s">
         <v>87</v>
       </c>
@@ -6671,11 +6674,11 @@
         <v>1E-4</v>
       </c>
       <c r="D22" s="28">
-        <f>0.9*C22</f>
+        <f t="shared" si="0"/>
         <v>9.0000000000000006E-5</v>
       </c>
       <c r="E22" s="28">
-        <f>1.1*C22</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000002E-4</v>
       </c>
       <c r="F22" s="27" t="s">
@@ -6687,7 +6690,7 @@
       <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="95"/>
+      <c r="A23" s="115"/>
       <c r="B23" s="25" t="s">
         <v>90</v>
       </c>
@@ -6695,11 +6698,11 @@
         <v>100</v>
       </c>
       <c r="D23" s="28">
-        <f>0.9*C23</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="E23" s="28">
-        <f>1.1*C23</f>
+        <f t="shared" si="1"/>
         <v>110.00000000000001</v>
       </c>
       <c r="F23" s="27" t="s">
@@ -6711,7 +6714,7 @@
       <c r="H23" s="49"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="96" t="s">
+      <c r="A24" s="116" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -6721,11 +6724,11 @@
         <v>0.63</v>
       </c>
       <c r="D24" s="12">
-        <f>0.9*C24</f>
+        <f t="shared" si="0"/>
         <v>0.56700000000000006</v>
       </c>
       <c r="E24" s="12">
-        <f>1.1*C24</f>
+        <f t="shared" si="1"/>
         <v>0.69300000000000006</v>
       </c>
       <c r="F24" s="7"/>
@@ -6735,7 +6738,7 @@
       <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="97"/>
+      <c r="A25" s="117"/>
       <c r="B25" s="9" t="s">
         <v>12</v>
       </c>
@@ -6743,11 +6746,11 @@
         <v>0.31</v>
       </c>
       <c r="D25" s="12">
-        <f>0.9*C25</f>
+        <f t="shared" si="0"/>
         <v>0.27900000000000003</v>
       </c>
       <c r="E25" s="12">
-        <f>1.1*C25</f>
+        <f t="shared" si="1"/>
         <v>0.34100000000000003</v>
       </c>
       <c r="F25" s="7"/>
@@ -6757,7 +6760,7 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="97"/>
+      <c r="A26" s="117"/>
       <c r="B26" s="9" t="s">
         <v>13</v>
       </c>
@@ -6765,11 +6768,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D26" s="12">
-        <f>0.9*C26</f>
+        <f t="shared" si="0"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E26" s="12">
-        <f>1.1*C26</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001E-5</v>
       </c>
       <c r="F26" s="7"/>
@@ -6779,7 +6782,7 @@
       <c r="H26" s="49"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="97"/>
+      <c r="A27" s="117"/>
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
@@ -6787,11 +6790,11 @@
         <v>0.06</v>
       </c>
       <c r="D27" s="12">
-        <f>0.9*C27</f>
+        <f t="shared" si="0"/>
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="E27" s="12">
-        <f>1.1*C27</f>
+        <f t="shared" si="1"/>
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="F27" s="7"/>
@@ -6801,7 +6804,7 @@
       <c r="H27" s="49"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="97"/>
+      <c r="A28" s="117"/>
       <c r="B28" s="9" t="s">
         <v>14</v>
       </c>
@@ -6809,11 +6812,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D28" s="12">
-        <f>0.9*C28</f>
+        <f t="shared" si="0"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E28" s="12">
-        <f>1.1*C28</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001E-5</v>
       </c>
       <c r="F28" s="7"/>
@@ -6823,7 +6826,7 @@
       <c r="H28" s="49"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="97"/>
+      <c r="A29" s="117"/>
       <c r="B29" s="9" t="s">
         <v>15</v>
       </c>
@@ -6831,11 +6834,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D29" s="12">
-        <f>0.9*C29</f>
+        <f t="shared" si="0"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E29" s="12">
-        <f>1.1*C29</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001E-5</v>
       </c>
       <c r="F29" s="7"/>
@@ -6845,7 +6848,7 @@
       <c r="H29" s="49"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="97"/>
+      <c r="A30" s="117"/>
       <c r="B30" s="36" t="s">
         <v>16</v>
       </c>
@@ -6853,11 +6856,11 @@
         <v>1.25</v>
       </c>
       <c r="D30" s="37">
-        <f>0.9*C30</f>
+        <f t="shared" si="0"/>
         <v>1.125</v>
       </c>
       <c r="E30" s="37">
-        <f>1.1*C30</f>
+        <f t="shared" si="1"/>
         <v>1.375</v>
       </c>
       <c r="F30" s="38"/>
@@ -6867,7 +6870,7 @@
       <c r="H30" s="49"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="97"/>
+      <c r="A31" s="117"/>
       <c r="B31" s="36" t="s">
         <v>17</v>
       </c>
@@ -6875,11 +6878,11 @@
         <v>1.25</v>
       </c>
       <c r="D31" s="37">
-        <f>0.9*C31</f>
+        <f t="shared" si="0"/>
         <v>1.125</v>
       </c>
       <c r="E31" s="37">
-        <f>1.1*C31</f>
+        <f t="shared" si="1"/>
         <v>1.375</v>
       </c>
       <c r="F31" s="38"/>
@@ -6889,7 +6892,7 @@
       <c r="H31" s="50"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="97"/>
+      <c r="A32" s="117"/>
       <c r="B32" s="36" t="s">
         <v>18</v>
       </c>
@@ -6897,11 +6900,11 @@
         <v>1</v>
       </c>
       <c r="D32" s="37">
-        <f>0.9*C32</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="E32" s="37">
-        <f>1.1*C32</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="F32" s="38"/>
@@ -6911,7 +6914,7 @@
       <c r="H32" s="50"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="97"/>
+      <c r="A33" s="117"/>
       <c r="B33" s="36" t="s">
         <v>22</v>
       </c>
@@ -6919,11 +6922,11 @@
         <v>1.2</v>
       </c>
       <c r="D33" s="37">
-        <f>0.9*C33</f>
+        <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
       <c r="E33" s="37">
-        <f>1.1*C33</f>
+        <f t="shared" si="1"/>
         <v>1.32</v>
       </c>
       <c r="F33" s="38"/>
@@ -6933,7 +6936,7 @@
       <c r="H33" s="80"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="97"/>
+      <c r="A34" s="117"/>
       <c r="B34" s="36" t="s">
         <v>19</v>
       </c>
@@ -6941,11 +6944,11 @@
         <v>1</v>
       </c>
       <c r="D34" s="37">
-        <f>0.9*C34</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="E34" s="37">
-        <f>1.1*C34</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="F34" s="38"/>
@@ -6955,7 +6958,7 @@
       <c r="H34" s="81"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="97"/>
+      <c r="A35" s="117"/>
       <c r="B35" s="36" t="s">
         <v>20</v>
       </c>
@@ -6963,11 +6966,11 @@
         <v>1</v>
       </c>
       <c r="D35" s="37">
-        <f>0.9*C35</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="E35" s="37">
-        <f>1.1*C35</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="F35" s="38"/>
@@ -6977,7 +6980,7 @@
       <c r="H35" s="81"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="100" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="51" t="s">
@@ -6988,11 +6991,11 @@
         <v>9990</v>
       </c>
       <c r="D36" s="52">
-        <f>0.9*C36</f>
+        <f t="shared" si="0"/>
         <v>8991</v>
       </c>
       <c r="E36" s="52">
-        <f>1.1*C36</f>
+        <f t="shared" si="1"/>
         <v>10989</v>
       </c>
       <c r="F36" s="53" t="s">
@@ -7004,7 +7007,7 @@
       <c r="H36" s="82"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="110"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="51" t="s">
         <v>27</v>
       </c>
@@ -7013,11 +7016,11 @@
         <v>9.99</v>
       </c>
       <c r="D37" s="52">
-        <f>0.9*C37</f>
+        <f t="shared" ref="D37:D68" si="2">0.9*C37</f>
         <v>8.9909999999999997</v>
       </c>
       <c r="E37" s="52">
-        <f>1.1*C37</f>
+        <f t="shared" ref="E37:E70" si="3">1.1*C37</f>
         <v>10.989000000000001</v>
       </c>
       <c r="F37" s="53" t="s">
@@ -7029,7 +7032,7 @@
       <c r="H37" s="80"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="110"/>
+      <c r="A38" s="101"/>
       <c r="B38" s="51" t="s">
         <v>28</v>
       </c>
@@ -7038,11 +7041,11 @@
         <v>8.01</v>
       </c>
       <c r="D38" s="52">
-        <f>0.9*C38</f>
+        <f t="shared" si="2"/>
         <v>7.2089999999999996</v>
       </c>
       <c r="E38" s="52">
-        <f>1.1*C38</f>
+        <f t="shared" si="3"/>
         <v>8.8109999999999999</v>
       </c>
       <c r="F38" s="53" t="s">
@@ -7054,7 +7057,7 @@
       <c r="H38" s="81"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="110"/>
+      <c r="A39" s="101"/>
       <c r="B39" s="51" t="s">
         <v>29</v>
       </c>
@@ -7063,11 +7066,11 @@
         <v>3.3750000000000002E-2</v>
       </c>
       <c r="D39" s="52">
-        <f>0.9*C39</f>
+        <f t="shared" si="2"/>
         <v>3.0375000000000003E-2</v>
       </c>
       <c r="E39" s="52">
-        <f>1.1*C39</f>
+        <f t="shared" si="3"/>
         <v>3.7125000000000005E-2</v>
       </c>
       <c r="F39" s="53" t="s">
@@ -7079,7 +7082,7 @@
       <c r="H39" s="81"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="111"/>
+      <c r="A40" s="102"/>
       <c r="B40" s="14" t="s">
         <v>165</v>
       </c>
@@ -7087,11 +7090,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D40" s="15">
-        <f>0.9*C40</f>
+        <f t="shared" si="2"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E40" s="15">
-        <f>1.1*C40</f>
+        <f t="shared" si="3"/>
         <v>1.1000000000000001E-5</v>
       </c>
       <c r="F40" s="16" t="s">
@@ -7103,7 +7106,7 @@
       <c r="H40" s="82"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="106" t="s">
+      <c r="A41" s="97" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="17" t="s">
@@ -7113,11 +7116,11 @@
         <v>330</v>
       </c>
       <c r="D41" s="18">
-        <f>0.9*C41</f>
+        <f t="shared" si="2"/>
         <v>297</v>
       </c>
       <c r="E41" s="18">
-        <f>1.1*C41</f>
+        <f t="shared" si="3"/>
         <v>363.00000000000006</v>
       </c>
       <c r="F41" s="19" t="s">
@@ -7129,7 +7132,7 @@
       <c r="H41" s="49"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="107"/>
+      <c r="A42" s="98"/>
       <c r="B42" s="17" t="s">
         <v>33</v>
       </c>
@@ -7137,11 +7140,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D42" s="18">
-        <f>0.9*C42</f>
+        <f t="shared" si="2"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E42" s="18">
-        <f>1.1*C42</f>
+        <f t="shared" si="3"/>
         <v>1.1000000000000001E-5</v>
       </c>
       <c r="F42" s="19" t="s">
@@ -7153,7 +7156,7 @@
       <c r="H42" s="49"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="107"/>
+      <c r="A43" s="98"/>
       <c r="B43" s="17" t="s">
         <v>34</v>
       </c>
@@ -7161,11 +7164,11 @@
         <v>2805</v>
       </c>
       <c r="D43" s="18">
-        <f>0.9*C43</f>
+        <f t="shared" si="2"/>
         <v>2524.5</v>
       </c>
       <c r="E43" s="18">
-        <f>1.1*C43</f>
+        <f t="shared" si="3"/>
         <v>3085.5000000000005</v>
       </c>
       <c r="F43" s="19" t="s">
@@ -7177,7 +7180,7 @@
       <c r="H43" s="49"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="107"/>
+      <c r="A44" s="98"/>
       <c r="B44" s="17" t="s">
         <v>35</v>
       </c>
@@ -7185,11 +7188,11 @@
         <v>0.03</v>
       </c>
       <c r="D44" s="18">
-        <f>0.9*C44</f>
+        <f t="shared" si="2"/>
         <v>2.7E-2</v>
       </c>
       <c r="E44" s="18">
-        <f>1.1*C44</f>
+        <f t="shared" si="3"/>
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="F44" s="19" t="s">
@@ -7201,7 +7204,7 @@
       <c r="H44" s="49"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="107"/>
+      <c r="A45" s="98"/>
       <c r="B45" s="17" t="s">
         <v>36</v>
       </c>
@@ -7209,11 +7212,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D45" s="18">
-        <f>0.9*C45</f>
+        <f t="shared" si="2"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E45" s="18">
-        <f>1.1*C45</f>
+        <f t="shared" si="3"/>
         <v>1.1000000000000001E-5</v>
       </c>
       <c r="F45" s="19" t="s">
@@ -7225,7 +7228,7 @@
       <c r="H45" s="49"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="107"/>
+      <c r="A46" s="98"/>
       <c r="B46" s="17" t="s">
         <v>37</v>
       </c>
@@ -7233,11 +7236,11 @@
         <v>2.44</v>
       </c>
       <c r="D46" s="18">
-        <f>0.9*C46</f>
+        <f t="shared" si="2"/>
         <v>2.1960000000000002</v>
       </c>
       <c r="E46" s="18">
-        <f>1.1*C46</f>
+        <f t="shared" si="3"/>
         <v>2.6840000000000002</v>
       </c>
       <c r="F46" s="19" t="s">
@@ -7249,7 +7252,7 @@
       <c r="H46" s="49"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="108"/>
+      <c r="A47" s="99"/>
       <c r="B47" s="17" t="s">
         <v>151</v>
       </c>
@@ -7257,11 +7260,11 @@
         <v>2805</v>
       </c>
       <c r="D47" s="18">
-        <f>0.9*C47</f>
+        <f t="shared" si="2"/>
         <v>2524.5</v>
       </c>
       <c r="E47" s="18">
-        <f>1.1*C47</f>
+        <f t="shared" si="3"/>
         <v>3085.5000000000005</v>
       </c>
       <c r="F47" s="19" t="s">
@@ -7273,7 +7276,7 @@
       <c r="H47" s="49"/>
     </row>
     <row r="48" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A48" s="118" t="s">
+      <c r="A48" s="89" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="20" t="s">
@@ -7284,11 +7287,11 @@
         <v>3.9115646258503403E-2</v>
       </c>
       <c r="D48" s="30">
-        <f>0.9*C48</f>
+        <f t="shared" si="2"/>
         <v>3.5204081632653067E-2</v>
       </c>
       <c r="E48" s="30">
-        <f>1.1*C48</f>
+        <f t="shared" si="3"/>
         <v>4.3027210884353746E-2</v>
       </c>
       <c r="F48" s="22" t="s">
@@ -7300,7 +7303,7 @@
       <c r="H48" s="49"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="119"/>
+      <c r="A49" s="90"/>
       <c r="B49" s="20" t="s">
         <v>171</v>
       </c>
@@ -7309,11 +7312,11 @@
         <v>0.76666666666666672</v>
       </c>
       <c r="D49" s="21">
-        <f>0.9*C49</f>
+        <f t="shared" si="2"/>
         <v>0.69000000000000006</v>
       </c>
       <c r="E49" s="21">
-        <f>1.1*C49</f>
+        <f t="shared" si="3"/>
         <v>0.84333333333333349</v>
       </c>
       <c r="F49" s="22" t="s">
@@ -7325,7 +7328,7 @@
       <c r="H49" s="80"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="119"/>
+      <c r="A50" s="90"/>
       <c r="B50" s="20" t="s">
         <v>173</v>
       </c>
@@ -7334,11 +7337,11 @@
         <v>0.15</v>
       </c>
       <c r="D50" s="21">
-        <f>0.9*C50</f>
+        <f t="shared" si="2"/>
         <v>0.13500000000000001</v>
       </c>
       <c r="E50" s="21">
-        <f>1.1*C50</f>
+        <f t="shared" si="3"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="F50" s="22" t="s">
@@ -7350,7 +7353,7 @@
       <c r="H50" s="81"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="119"/>
+      <c r="A51" s="90"/>
       <c r="B51" s="20" t="s">
         <v>213</v>
       </c>
@@ -7359,11 +7362,11 @@
         <v>0.15305300467214436</v>
       </c>
       <c r="D51" s="21">
-        <f>0.9*C51</f>
+        <f t="shared" si="2"/>
         <v>0.13774770420492993</v>
       </c>
       <c r="E51" s="21">
-        <f>1.1*C51</f>
+        <f t="shared" si="3"/>
         <v>0.16835830513935882</v>
       </c>
       <c r="F51" s="22" t="s">
@@ -7375,7 +7378,7 @@
       <c r="H51" s="81"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="119"/>
+      <c r="A52" s="90"/>
       <c r="B52" s="20" t="s">
         <v>212</v>
       </c>
@@ -7384,11 +7387,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D52" s="21">
-        <f>0.9*C52</f>
+        <f t="shared" si="2"/>
         <v>1.35E-2</v>
       </c>
       <c r="E52" s="21">
-        <f>1.1*C52</f>
+        <f t="shared" si="3"/>
         <v>1.6500000000000001E-2</v>
       </c>
       <c r="F52" s="22" t="s">
@@ -7400,7 +7403,7 @@
       <c r="H52" s="81"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="119"/>
+      <c r="A53" s="90"/>
       <c r="B53" s="20" t="s">
         <v>217</v>
       </c>
@@ -7409,11 +7412,11 @@
         <v>882</v>
       </c>
       <c r="D53" s="21">
-        <f>0.9*C53</f>
+        <f t="shared" si="2"/>
         <v>793.80000000000007</v>
       </c>
       <c r="E53" s="21">
-        <f>1.1*C53</f>
+        <f t="shared" si="3"/>
         <v>970.2</v>
       </c>
       <c r="F53" s="22" t="s">
@@ -7425,7 +7428,7 @@
       <c r="H53" s="81"/>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="119"/>
+      <c r="A54" s="90"/>
       <c r="B54" s="20" t="s">
         <v>170</v>
       </c>
@@ -7433,11 +7436,11 @@
         <v>30</v>
       </c>
       <c r="D54" s="21">
-        <f>0.9*C54</f>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="E54" s="21">
-        <f>1.1*C54</f>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="F54" s="22" t="s">
@@ -7449,7 +7452,7 @@
       <c r="H54" s="81"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="119"/>
+      <c r="A55" s="90"/>
       <c r="B55" s="20" t="s">
         <v>174</v>
       </c>
@@ -7457,11 +7460,11 @@
         <v>60</v>
       </c>
       <c r="D55" s="21">
-        <f>0.9*C55</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="E55" s="21">
-        <f>1.1*C55</f>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="F55" s="22" t="s">
@@ -7473,7 +7476,7 @@
       <c r="H55" s="81"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="119"/>
+      <c r="A56" s="90"/>
       <c r="B56" s="23" t="s">
         <v>208</v>
       </c>
@@ -7482,11 +7485,11 @@
         <v>62.07</v>
       </c>
       <c r="D56" s="21">
-        <f>0.9*C56</f>
+        <f t="shared" si="2"/>
         <v>55.863</v>
       </c>
       <c r="E56" s="21">
-        <f>1.1*C56</f>
+        <f t="shared" si="3"/>
         <v>68.277000000000001</v>
       </c>
       <c r="F56" s="22" t="s">
@@ -7498,7 +7501,7 @@
       <c r="H56" s="81"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="119"/>
+      <c r="A57" s="90"/>
       <c r="B57" s="23" t="s">
         <v>209</v>
       </c>
@@ -7506,11 +7509,11 @@
         <v>600</v>
       </c>
       <c r="D57" s="21">
-        <f>0.9*C57</f>
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
       <c r="E57" s="21">
-        <f>1.1*C57</f>
+        <f t="shared" si="3"/>
         <v>660</v>
       </c>
       <c r="F57" s="22" t="s">
@@ -7522,7 +7525,7 @@
       <c r="H57" s="81"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="119"/>
+      <c r="A58" s="90"/>
       <c r="B58" s="23" t="s">
         <v>163</v>
       </c>
@@ -7530,11 +7533,11 @@
         <v>4.3</v>
       </c>
       <c r="D58" s="21">
-        <f>0.9*C58</f>
+        <f t="shared" si="2"/>
         <v>3.87</v>
       </c>
       <c r="E58" s="21">
-        <f>1.1*C58</f>
+        <f t="shared" si="3"/>
         <v>4.7300000000000004</v>
       </c>
       <c r="F58" s="24" t="s">
@@ -7546,7 +7549,7 @@
       <c r="H58" s="82"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="119"/>
+      <c r="A59" s="90"/>
       <c r="B59" s="23" t="s">
         <v>164</v>
       </c>
@@ -7555,11 +7558,11 @@
         <v>0.81</v>
       </c>
       <c r="D59" s="21">
-        <f>0.9*C59</f>
+        <f t="shared" si="2"/>
         <v>0.72900000000000009</v>
       </c>
       <c r="E59" s="21">
-        <f>1.1*C59</f>
+        <f t="shared" si="3"/>
         <v>0.89100000000000013</v>
       </c>
       <c r="F59" s="24"/>
@@ -7569,7 +7572,7 @@
       <c r="H59" s="49"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="119"/>
+      <c r="A60" s="90"/>
       <c r="B60" s="23" t="s">
         <v>221</v>
       </c>
@@ -7577,11 +7580,11 @@
         <v>10</v>
       </c>
       <c r="D60" s="21">
-        <f>0.9*C60</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="E60" s="21">
-        <f>1.1*C60</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="F60" s="24"/>
@@ -7591,7 +7594,7 @@
       <c r="H60" s="73"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="119"/>
+      <c r="A61" s="90"/>
       <c r="B61" s="41" t="s">
         <v>41</v>
       </c>
@@ -7599,11 +7602,11 @@
         <v>2.3315789473684214</v>
       </c>
       <c r="D61" s="42">
-        <f>0.9*C61</f>
+        <f t="shared" si="2"/>
         <v>2.0984210526315792</v>
       </c>
       <c r="E61" s="42">
-        <f>1.1*C61</f>
+        <f t="shared" si="3"/>
         <v>2.5647368421052636</v>
       </c>
       <c r="F61" s="43" t="s">
@@ -7615,7 +7618,7 @@
       <c r="H61" s="80"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="119"/>
+      <c r="A62" s="90"/>
       <c r="B62" s="41" t="s">
         <v>42</v>
       </c>
@@ -7623,11 +7626,11 @@
         <v>4.4784688995215309E-2</v>
       </c>
       <c r="D62" s="42">
-        <f>0.9*C62</f>
+        <f t="shared" si="2"/>
         <v>4.0306220095693776E-2</v>
       </c>
       <c r="E62" s="42">
-        <f>1.1*C62</f>
+        <f t="shared" si="3"/>
         <v>4.9263157894736842E-2</v>
       </c>
       <c r="F62" s="43" t="s">
@@ -7639,7 +7642,7 @@
       <c r="H62" s="81"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="119"/>
+      <c r="A63" s="90"/>
       <c r="B63" s="41" t="s">
         <v>92</v>
       </c>
@@ -7647,11 +7650,11 @@
         <v>4.2497607655502394</v>
       </c>
       <c r="D63" s="42">
-        <f>0.9*C63</f>
+        <f t="shared" si="2"/>
         <v>3.8247846889952157</v>
       </c>
       <c r="E63" s="42">
-        <f>1.1*C63</f>
+        <f t="shared" si="3"/>
         <v>4.674736842105264</v>
       </c>
       <c r="F63" s="43" t="s">
@@ -7663,7 +7666,7 @@
       <c r="H63" s="81"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="119"/>
+      <c r="A64" s="90"/>
       <c r="B64" s="41" t="s">
         <v>93</v>
       </c>
@@ -7671,11 +7674,11 @@
         <v>6</v>
       </c>
       <c r="D64" s="42">
-        <f>0.9*C64</f>
+        <f t="shared" si="2"/>
         <v>5.4</v>
       </c>
       <c r="E64" s="42">
-        <f>1.1*C64</f>
+        <f t="shared" si="3"/>
         <v>6.6000000000000005</v>
       </c>
       <c r="F64" s="43" t="s">
@@ -7687,7 +7690,7 @@
       <c r="H64" s="82"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="120"/>
+      <c r="A65" s="91"/>
       <c r="B65" s="41" t="s">
         <v>225</v>
       </c>
@@ -7695,11 +7698,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D65" s="42">
-        <f>0.9*C65</f>
+        <f t="shared" si="2"/>
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="E65" s="42">
-        <f>1.1*C65</f>
+        <f t="shared" si="3"/>
         <v>1.1000000000000001E-5</v>
       </c>
       <c r="F65" s="43"/>
@@ -7709,7 +7712,7 @@
       <c r="H65" s="81"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="89" t="s">
+      <c r="A66" s="109" t="s">
         <v>49</v>
       </c>
       <c r="B66" s="55" t="s">
@@ -7719,11 +7722,11 @@
         <v>0.25</v>
       </c>
       <c r="D66" s="76">
-        <f>0.9*C66</f>
+        <f t="shared" si="2"/>
         <v>0.22500000000000001</v>
       </c>
       <c r="E66" s="76">
-        <f>1.1*C66</f>
+        <f t="shared" si="3"/>
         <v>0.27500000000000002</v>
       </c>
       <c r="F66" s="56"/>
@@ -7733,7 +7736,7 @@
       <c r="H66" s="83"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="90"/>
+      <c r="A67" s="110"/>
       <c r="B67" s="55" t="s">
         <v>59</v>
       </c>
@@ -7741,11 +7744,11 @@
         <v>0.2</v>
       </c>
       <c r="D67" s="76">
-        <f>0.9*C67</f>
+        <f t="shared" si="2"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="E67" s="76">
-        <f>1.1*C67</f>
+        <f t="shared" si="3"/>
         <v>0.22000000000000003</v>
       </c>
       <c r="F67" s="56"/>
@@ -7755,7 +7758,7 @@
       <c r="H67" s="84"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="90"/>
+      <c r="A68" s="110"/>
       <c r="B68" s="55" t="s">
         <v>51</v>
       </c>
@@ -7763,11 +7766,11 @@
         <v>0.2</v>
       </c>
       <c r="D68" s="76">
-        <f>0.9*C68</f>
+        <f t="shared" si="2"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="E68" s="76">
-        <f>1.1*C68</f>
+        <f t="shared" si="3"/>
         <v>0.22000000000000003</v>
       </c>
       <c r="F68" s="56"/>
@@ -7777,7 +7780,7 @@
       <c r="H68" s="84"/>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="90"/>
+      <c r="A69" s="110"/>
       <c r="B69" s="55" t="s">
         <v>52</v>
       </c>
@@ -7785,11 +7788,11 @@
         <v>0.2</v>
       </c>
       <c r="D69" s="76">
-        <f>0.9*C69</f>
+        <f t="shared" ref="D69:D100" si="4">0.9*C69</f>
         <v>0.18000000000000002</v>
       </c>
       <c r="E69" s="76">
-        <f>1.1*C69</f>
+        <f t="shared" si="3"/>
         <v>0.22000000000000003</v>
       </c>
       <c r="F69" s="56"/>
@@ -7799,7 +7802,7 @@
       <c r="H69" s="84"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="90"/>
+      <c r="A70" s="110"/>
       <c r="B70" s="55" t="s">
         <v>53</v>
       </c>
@@ -7807,11 +7810,11 @@
         <v>0.5</v>
       </c>
       <c r="D70" s="76">
-        <f>0.9*C70</f>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="E70" s="76">
-        <f>1.1*C70</f>
+        <f t="shared" si="3"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="F70" s="56"/>
@@ -7821,7 +7824,7 @@
       <c r="H70" s="84"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="90"/>
+      <c r="A71" s="110"/>
       <c r="B71" s="55" t="s">
         <v>94</v>
       </c>
@@ -7829,11 +7832,11 @@
         <v>0.5</v>
       </c>
       <c r="D71" s="76">
-        <f t="shared" ref="D71:D83" si="0">0.9*C71</f>
+        <f t="shared" ref="D71:D83" si="5">0.9*C71</f>
         <v>0.45</v>
       </c>
       <c r="E71" s="76">
-        <f t="shared" ref="E71:E83" si="1">1.1*C71</f>
+        <f t="shared" ref="E71:E83" si="6">1.1*C71</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="F71" s="56"/>
@@ -7843,7 +7846,7 @@
       <c r="H71" s="84"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="90"/>
+      <c r="A72" s="110"/>
       <c r="B72" s="55" t="s">
         <v>54</v>
       </c>
@@ -7851,11 +7854,11 @@
         <v>0.25</v>
       </c>
       <c r="D72" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.22500000000000001</v>
       </c>
       <c r="E72" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.27500000000000002</v>
       </c>
       <c r="F72" s="56"/>
@@ -7865,7 +7868,7 @@
       <c r="H72" s="84"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="90"/>
+      <c r="A73" s="110"/>
       <c r="B73" s="55" t="s">
         <v>60</v>
       </c>
@@ -7873,11 +7876,11 @@
         <v>0.1</v>
       </c>
       <c r="D73" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="E73" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.11000000000000001</v>
       </c>
       <c r="F73" s="56"/>
@@ -7887,7 +7890,7 @@
       <c r="H73" s="84"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="90"/>
+      <c r="A74" s="110"/>
       <c r="B74" s="55" t="s">
         <v>55</v>
       </c>
@@ -7895,11 +7898,11 @@
         <v>0.1</v>
       </c>
       <c r="D74" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="E74" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.11000000000000001</v>
       </c>
       <c r="F74" s="56"/>
@@ -7909,7 +7912,7 @@
       <c r="H74" s="84"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="90"/>
+      <c r="A75" s="110"/>
       <c r="B75" s="55" t="s">
         <v>56</v>
       </c>
@@ -7917,11 +7920,11 @@
         <v>0.1</v>
       </c>
       <c r="D75" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="E75" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.11000000000000001</v>
       </c>
       <c r="F75" s="56"/>
@@ -7931,7 +7934,7 @@
       <c r="H75" s="84"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="90"/>
+      <c r="A76" s="110"/>
       <c r="B76" s="55" t="s">
         <v>57</v>
       </c>
@@ -7939,11 +7942,11 @@
         <v>0.45</v>
       </c>
       <c r="D76" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.40500000000000003</v>
       </c>
       <c r="E76" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.49500000000000005</v>
       </c>
       <c r="F76" s="56"/>
@@ -7953,7 +7956,7 @@
       <c r="H76" s="84"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="90"/>
+      <c r="A77" s="110"/>
       <c r="B77" s="55" t="s">
         <v>96</v>
       </c>
@@ -7961,11 +7964,11 @@
         <v>0.45</v>
       </c>
       <c r="D77" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.40500000000000003</v>
       </c>
       <c r="E77" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.49500000000000005</v>
       </c>
       <c r="F77" s="56"/>
@@ -7975,7 +7978,7 @@
       <c r="H77" s="84"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="90"/>
+      <c r="A78" s="110"/>
       <c r="B78" s="55" t="s">
         <v>58</v>
       </c>
@@ -7983,11 +7986,11 @@
         <v>0.5</v>
       </c>
       <c r="D78" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.45</v>
       </c>
       <c r="E78" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="F78" s="56"/>
@@ -7997,7 +8000,7 @@
       <c r="H78" s="84"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="90"/>
+      <c r="A79" s="110"/>
       <c r="B79" s="55" t="s">
         <v>61</v>
       </c>
@@ -8005,11 +8008,11 @@
         <v>0.7</v>
       </c>
       <c r="D79" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.63</v>
       </c>
       <c r="E79" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.77</v>
       </c>
       <c r="F79" s="56"/>
@@ -8019,7 +8022,7 @@
       <c r="H79" s="84"/>
     </row>
     <row r="80" spans="1:8">
-      <c r="A80" s="90"/>
+      <c r="A80" s="110"/>
       <c r="B80" s="55" t="s">
         <v>62</v>
       </c>
@@ -8027,11 +8030,11 @@
         <v>0.7</v>
       </c>
       <c r="D80" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.63</v>
       </c>
       <c r="E80" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.77</v>
       </c>
       <c r="F80" s="56"/>
@@ -8041,7 +8044,7 @@
       <c r="H80" s="84"/>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="90"/>
+      <c r="A81" s="110"/>
       <c r="B81" s="55" t="s">
         <v>63</v>
       </c>
@@ -8049,11 +8052,11 @@
         <v>0.7</v>
       </c>
       <c r="D81" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.63</v>
       </c>
       <c r="E81" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.77</v>
       </c>
       <c r="F81" s="56"/>
@@ -8063,7 +8066,7 @@
       <c r="H81" s="84"/>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="90"/>
+      <c r="A82" s="110"/>
       <c r="B82" s="55" t="s">
         <v>64</v>
       </c>
@@ -8071,11 +8074,11 @@
         <v>0.05</v>
       </c>
       <c r="D82" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.5000000000000005E-2</v>
       </c>
       <c r="E82" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>5.5000000000000007E-2</v>
       </c>
       <c r="F82" s="56"/>
@@ -8085,7 +8088,7 @@
       <c r="H82" s="84"/>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="90"/>
+      <c r="A83" s="110"/>
       <c r="B83" s="55" t="s">
         <v>95</v>
       </c>
@@ -8093,11 +8096,11 @@
         <v>0.05</v>
       </c>
       <c r="D83" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.5000000000000005E-2</v>
       </c>
       <c r="E83" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>5.5000000000000007E-2</v>
       </c>
       <c r="F83" s="56"/>
@@ -8131,12 +8134,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8363,15 +8363,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9031FEDD-5FF8-4C9C-AF51-AEFA4BF396D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145C285F-2FF3-4D38-95ED-9BA60F4E3C89}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="47151ffa-27c1-491d-bdc5-fff6d8a44614"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2a729546-cf4e-435c-aabc-21366d2421e1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8396,18 +8408,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145C285F-2FF3-4D38-95ED-9BA60F4E3C89}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9031FEDD-5FF8-4C9C-AF51-AEFA4BF396D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="47151ffa-27c1-491d-bdc5-fff6d8a44614"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2a729546-cf4e-435c-aabc-21366d2421e1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>